<commit_message>
Activity 1 W05 done
</commit_message>
<xml_diff>
--- a/MATH 108X/GroupAssignment -Budgeting_a - W0.xlsx
+++ b/MATH 108X/GroupAssignment -Budgeting_a - W0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Leti\Programming\MATH 108X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAABCFC-A324-439E-B5CF-6B2067DCA0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E214A22-773E-46B8-A1E1-3575EFA90DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1274,14 +1274,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="2" borderId="49" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="6" fontId="11" fillId="2" borderId="15" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="8" fontId="11" fillId="2" borderId="15" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="11" fillId="2" borderId="15" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="8" fontId="11" fillId="2" borderId="15" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
@@ -2464,6 +2464,14 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>No, it leaves him</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> with little money for groceries and no monthly cash flow. I would lessen the entertainment budget to 20 dollars leaving 35 dollars extra for groceries. I would also get a phone that costs less and use the extra money from that to be the monthly cash flow.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -3051,6 +3059,14 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>She could reduce</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> the groceries to 225 and have 30 dollars for entertainment with the extra 34 dollars as the monthly cash flow. Her new goal is nor reasonable because she has no monthly cash flow and not a lot for entertainment.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -3823,6 +3839,14 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Sticking with</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> the one year cell phone plan will be cheaper because if they pay for any of the monthly plans it will end up costing more than the annual $495 and with the same benefits of the last three plans and more than the all you need plan.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -4097,8 +4121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -4122,9 +4146,9 @@
     </row>
     <row r="4" spans="2:7" ht="43.05" customHeight="1">
       <c r="B4" s="1"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
@@ -4153,8 +4177,8 @@
       <c r="E7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="104">
-        <v>628</v>
+      <c r="F7" s="102">
+        <v>314</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -4165,7 +4189,7 @@
       <c r="E8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="104">
+      <c r="F8" s="102">
         <v>628</v>
       </c>
       <c r="G8" s="1"/>
@@ -4195,7 +4219,7 @@
       <c r="E11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="105">
+      <c r="F11" s="103">
         <v>62.8</v>
       </c>
       <c r="G11" s="1"/>
@@ -4207,7 +4231,7 @@
       <c r="E12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="105">
+      <c r="F12" s="103">
         <v>94.2</v>
       </c>
       <c r="G12" s="1"/>
@@ -4219,8 +4243,8 @@
       <c r="E13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="105">
-        <v>115.26</v>
+      <c r="F13" s="103">
+        <v>212.34</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -4231,7 +4255,7 @@
       <c r="E14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="105">
+      <c r="F14" s="103">
         <v>59.99</v>
       </c>
       <c r="G14" s="1"/>
@@ -4243,7 +4267,7 @@
       <c r="E15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="105">
+      <c r="F15" s="103">
         <v>39.549999999999997</v>
       </c>
       <c r="G15" s="1"/>
@@ -4255,9 +4279,9 @@
       <c r="E16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="105">
+      <c r="F16" s="103">
         <f>SUM(F11:F15)</f>
-        <v>371.8</v>
+        <v>468.88000000000005</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -4298,8 +4322,8 @@
       <c r="E20" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="41">
-        <v>371</v>
+      <c r="F20" s="103">
+        <v>468.88</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -4311,7 +4335,8 @@
         <v>13</v>
       </c>
       <c r="F21" s="41">
-        <v>257</v>
+        <f>F19-F20</f>
+        <v>159.12</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -4344,8 +4369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -4529,7 +4554,10 @@
       <c r="E17" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="63"/>
+      <c r="F17" s="63">
+        <f>SUM(F12:F16)</f>
+        <v>225</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:7" ht="21.6" thickBot="1">
@@ -4918,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -5013,7 +5041,9 @@
       <c r="E8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="75"/>
+      <c r="F8" s="75">
+        <v>181</v>
+      </c>
       <c r="G8" s="70">
         <v>0</v>
       </c>
@@ -5029,7 +5059,7 @@
       </c>
       <c r="F9" s="76">
         <f>SUM(F7:F8)</f>
-        <v>450</v>
+        <v>631</v>
       </c>
       <c r="G9" s="77">
         <f>SUM(G7:G8)</f>
@@ -5136,7 +5166,9 @@
       <c r="F16" s="78">
         <v>75</v>
       </c>
-      <c r="G16" s="79"/>
+      <c r="G16" s="79">
+        <v>9</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
@@ -5153,7 +5185,7 @@
       </c>
       <c r="G17" s="77">
         <f>SUM(G12:G16)</f>
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -5191,7 +5223,7 @@
       </c>
       <c r="F20" s="81">
         <f>F9</f>
-        <v>450</v>
+        <v>631</v>
       </c>
       <c r="G20" s="68">
         <f>G7</f>
@@ -5213,7 +5245,7 @@
       </c>
       <c r="G21" s="83">
         <f>G17</f>
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -5227,11 +5259,11 @@
       </c>
       <c r="F22" s="84">
         <f>F20-F21</f>
-        <v>-181</v>
+        <v>0</v>
       </c>
       <c r="G22" s="77">
         <f>G20-G21</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -5715,8 +5747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="95" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -5986,10 +6018,10 @@
     <row r="22" spans="2:11">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="103" t="s">
+      <c r="D22" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="103"/>
+      <c r="E22" s="105"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -5999,8 +6031,8 @@
     <row r="23" spans="2:11">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -6010,8 +6042,8 @@
     <row r="24" spans="2:11" ht="24" customHeight="1">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -6055,8 +6087,12 @@
       <c r="G27" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="87"/>
-      <c r="I27" s="86"/>
+      <c r="H27" s="87">
+        <v>495</v>
+      </c>
+      <c r="I27" s="86">
+        <v>41.25</v>
+      </c>
       <c r="J27" s="9"/>
       <c r="K27" s="7"/>
     </row>
@@ -6069,8 +6105,12 @@
       <c r="G28" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="45"/>
-      <c r="I28" s="86"/>
+      <c r="H28" s="45">
+        <v>510</v>
+      </c>
+      <c r="I28" s="86">
+        <v>42.5</v>
+      </c>
       <c r="J28" s="10"/>
       <c r="K28" s="8"/>
     </row>
@@ -6083,8 +6123,12 @@
       <c r="G29" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="45"/>
-      <c r="I29" s="86"/>
+      <c r="H29" s="45">
+        <v>390</v>
+      </c>
+      <c r="I29" s="86">
+        <v>32.5</v>
+      </c>
       <c r="J29" s="10"/>
       <c r="K29" s="8"/>
     </row>
@@ -6097,8 +6141,12 @@
       <c r="G30" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="45"/>
-      <c r="I30" s="86"/>
+      <c r="H30" s="45">
+        <v>540</v>
+      </c>
+      <c r="I30" s="86">
+        <v>45</v>
+      </c>
       <c r="J30" s="10"/>
       <c r="K30" s="8"/>
     </row>
@@ -6111,8 +6159,12 @@
       <c r="G31" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="45"/>
-      <c r="I31" s="86"/>
+      <c r="H31" s="45">
+        <v>360</v>
+      </c>
+      <c r="I31" s="86">
+        <v>30</v>
+      </c>
       <c r="J31" s="10"/>
       <c r="K31" s="8"/>
     </row>

</xml_diff>